<commit_message>
fix weird format again
</commit_message>
<xml_diff>
--- a/Raw Input Data/Processing/Case 21/Suspect transaction record.xlsx
+++ b/Raw Input Data/Processing/Case 21/Suspect transaction record.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hbap.adroot.hsbc\HK\HASE\28062201\Fraud_Ops_FIM_File_Sharing\HASE case\Gen AI\Upload to sharepoint\Batch 2\Case 21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Processing\Case 21\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF67A3C-BAD9-4B0F-8178-231990130CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="14018"/>
+    <workbookView xWindow="-26070" yWindow="6810" windowWidth="20520" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction record" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="34">
   <si>
     <t>Transaction Date (value)</t>
   </si>
@@ -131,9 +121,6 @@
   </si>
   <si>
     <t>333-333333-101</t>
-  </si>
-  <si>
-    <t>\</t>
   </si>
   <si>
     <t>CHAN TAI MAN</t>
@@ -145,11 +132,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,29 +540,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="22.3125" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="18.8125" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
-    <col min="10" max="10" width="28.5" customWidth="1"/>
-    <col min="11" max="11" width="19.875" customWidth="1"/>
-    <col min="12" max="12" width="13.3125" customWidth="1"/>
-    <col min="15" max="15" width="48.625" customWidth="1"/>
-    <col min="16" max="16" width="18.1875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="48.5703125" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.9">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -628,7 +615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="2" customFormat="1">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45629</v>
       </c>
@@ -636,7 +623,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -678,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="2" customFormat="1">
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45629</v>
       </c>
@@ -686,7 +673,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>31</v>
@@ -728,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="2" customFormat="1">
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45629</v>
       </c>
@@ -736,7 +723,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>31</v>
@@ -778,7 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="2" customFormat="1">
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45629</v>
       </c>
@@ -786,7 +773,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>31</v>
@@ -828,7 +815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="2" customFormat="1">
+    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45629</v>
       </c>
@@ -836,7 +823,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>31</v>
@@ -878,7 +865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="2" customFormat="1">
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45629</v>
       </c>
@@ -886,7 +873,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>31</v>
@@ -928,7 +915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45629</v>
       </c>
@@ -936,7 +923,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>31</v>
@@ -978,7 +965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="2" customFormat="1">
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45629</v>
       </c>
@@ -986,7 +973,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
@@ -1028,7 +1015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="2" customFormat="1">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45629</v>
       </c>
@@ -1036,7 +1023,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -1078,7 +1065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45629</v>
       </c>
@@ -1086,7 +1073,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>31</v>
@@ -1128,7 +1115,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="2" customFormat="1">
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45629</v>
       </c>
@@ -1136,7 +1123,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>31</v>
@@ -1178,7 +1165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="2" customFormat="1">
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45629</v>
       </c>
@@ -1186,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>31</v>
@@ -1228,7 +1215,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="2" customFormat="1">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45629</v>
       </c>
@@ -1239,7 +1226,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
@@ -1254,7 +1241,7 @@
         <v>27</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>24</v>
@@ -1272,7 +1259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="2" customFormat="1">
+    <row r="15" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45629</v>
       </c>
@@ -1320,11 +1307,6 @@
       </c>
       <c r="Q15" s="2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="14:14">
-      <c r="N60" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1337,6 +1319,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A8F4FDE63F23240996C0B5ED71CAB02" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61b2ee7a38442529347de99e33b69841">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc14db02-3d39-436b-9056-63d1dbe054e8" xmlns:ns3="5ed3fcfa-dd51-4f96-90c6-6669337cd654" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="405649729e347460199c909c216f19f3" ns2:_="" ns3:_="">
     <xsd:import namespace="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
@@ -1531,34 +1533,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13E8F2EA-D8D4-4337-ADF1-8C1A0F32602C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97604FE5-0447-41C2-9BAF-DDE6C4F1D8A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0C1301E-DE77-4676-B64E-F1209C6B22A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0C1301E-DE77-4676-B64E-F1209C6B22A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97604FE5-0447-41C2-9BAF-DDE6C4F1D8A8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13E8F2EA-D8D4-4337-ADF1-8C1A0F32602C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>